<commit_message>
david modify vcs code
</commit_message>
<xml_diff>
--- a/_2.vcs/______test_files/__RW/_excel/vcs_ReadWrite_EXCEL7_Items.xlsx
+++ b/_2.vcs/______test_files/__RW/_excel/vcs_ReadWrite_EXCEL7_Items.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20730" windowHeight="9495" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20730" windowHeight="9495" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="11-09-14" sheetId="4" r:id="rId4"/>
     <sheet name="12-31-20" sheetId="5" r:id="rId5"/>
     <sheet name="02-17-21" sheetId="6" r:id="rId6"/>
+    <sheet name="08-01-22" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>A</t>
   </si>
@@ -44,6 +45,10 @@
   </si>
   <si>
     <t>C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -599,13 +604,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>

</xml_diff>